<commit_message>
better diagram for tunneling
</commit_message>
<xml_diff>
--- a/img/excel/diagrams.xlsx
+++ b/img/excel/diagrams.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubahronik\Desktop\Thesis\img\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE5D30A-9992-4C9F-A652-30C76FBB4628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600BE8B-9D19-4666-A605-2FAF61EF87D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{23EAE5E5-F549-4271-837A-78A13B533C97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{23EAE5E5-F549-4271-837A-78A13B533C97}"/>
   </bookViews>
   <sheets>
     <sheet name="swordPositioning" sheetId="1" r:id="rId1"/>
     <sheet name="slashingMode" sheetId="2" r:id="rId2"/>
+    <sheet name="tunneling" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1476,6 +1477,457 @@
             <a:rPr lang="cs-CZ" sz="2000"/>
             <a:t>3.</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Obdélník 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A8BD072-9290-4C80-B52A-85C4F0AAAFEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="31750"/>
+          <a:ext cx="2952750" cy="3854450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="41275">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Obdélník 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E67443D-85B4-472C-9E57-0AAB494DE369}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4851400" y="2165350"/>
+          <a:ext cx="552450" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="41275">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Přímá spojnice se šipkou 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC9799CE-3A26-109B-3775-74C6AE2D9D3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="933450"/>
+          <a:ext cx="4622800" cy="1174750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Přímá spojnice se šipkou 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93583BEF-BF97-469C-AB16-315DF6FF25AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="196850" y="2063750"/>
+          <a:ext cx="4629150" cy="1212850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextovéPole 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B782EF-9563-1248-1E57-0DF2BE3B8C15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="488950"/>
+          <a:ext cx="1009650" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="1800"/>
+            <a:t>Frame N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextovéPole 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7819700F-65DE-49AC-B98C-AFE1C276C249}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4622800" y="1593850"/>
+          <a:ext cx="1257300" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="1800"/>
+            <a:t>Frame N+1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Obdélník 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C46CBBB8-059F-4464-8F03-7F48E2F4177E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="203200" y="920750"/>
+          <a:ext cx="552450" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="41275">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1799,7 +2251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C24C4CB-874C-4BC7-A7BF-14B239817CA9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -1808,4 +2260,19 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5E9BC4-1613-4D8F-908A-F7A6847BDABE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
5.2.3 wip - up to finding shortest connection
</commit_message>
<xml_diff>
--- a/img/excel/diagrams.xlsx
+++ b/img/excel/diagrams.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubahronik\Desktop\Thesis\img\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600BE8B-9D19-4666-A605-2FAF61EF87D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501B599F-AE9A-4FF8-9870-E5C32FF9BA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{23EAE5E5-F549-4271-837A-78A13B533C97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{23EAE5E5-F549-4271-837A-78A13B533C97}"/>
   </bookViews>
   <sheets>
     <sheet name="swordPositioning" sheetId="1" r:id="rId1"/>
     <sheet name="slashingMode" sheetId="2" r:id="rId2"/>
     <sheet name="tunneling" sheetId="3" r:id="rId3"/>
+    <sheet name="fixer2D" sheetId="4" r:id="rId4"/>
+    <sheet name="fixer2D (2)" sheetId="6" r:id="rId5"/>
+    <sheet name="fixerDefinitions" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1931,6 +1934,1220 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>262380</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438418</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>118440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Obdélník 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94CE91D7-39C9-7E5B-EDFC-273BD7DF9429}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1896997">
+          <a:off x="262380" y="253625"/>
+          <a:ext cx="786258" cy="778595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>111512</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>273311</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>40269</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Přímá spojnice 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28EFF2E6-1CAD-09B6-BBDB-57699E28C5DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="12" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="111512" y="310161"/>
+          <a:ext cx="1992458" cy="461132"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>435565</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>86257</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>586629</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52063</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Ovál 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA20529-4645-5774-985D-25332AD9CCE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1045785" y="451769"/>
+          <a:ext cx="151064" cy="148562"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>269988</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>421410</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>182066</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Ovál 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{937299A4-D854-475C-9DD4-22A8F465E29A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1757291">
+          <a:off x="2100647" y="216258"/>
+          <a:ext cx="151422" cy="148564"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="C00000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>262380</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438418</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>118440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Obdélník 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6402CFC0-7F85-4DCF-995C-C9DC8FACE0A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1896997">
+          <a:off x="262380" y="255019"/>
+          <a:ext cx="785638" cy="784171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>53474</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>273311</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>93579</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Přímá spojnice 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A42F3256-8817-4C3F-A731-35AD17A3E9E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="5" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="661737" y="311221"/>
+          <a:ext cx="1436363" cy="333805"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>435565</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>86257</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>586629</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52063</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Ovál 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B19B6128-9E1D-4968-B09D-3982F44CC005}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1045165" y="454557"/>
+          <a:ext cx="151064" cy="149956"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>269988</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>421410</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>182066</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Ovál 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19B37C4D-3E8E-4DE3-A9CE-5B786FB7AE4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1757291">
+          <a:off x="2098788" y="217652"/>
+          <a:ext cx="151422" cy="148564"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="C00000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>603889</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obrázek 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE3437E0-04B1-DF7D-FC45-485AAB4E572A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3042289" cy="4184650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>51594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>178593</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>134938</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Pravá složená závorka 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EADE6654-3F61-45BC-1BD2-5EA5A87FF91B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2936875" y="51594"/>
+          <a:ext cx="297656" cy="3369469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 32333"/>
+            <a:gd name="adj2" fmla="val 50118"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353218</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>396875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Přímá spojnice 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33CAC4F1-0831-BEC4-C899-612D576275AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="964406" y="3397250"/>
+          <a:ext cx="1266032" cy="682625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>261938</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>472281</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Přímá spojnice 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4E25475-5EBE-4C71-A596-E038D70C848A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="261938" y="3405188"/>
+          <a:ext cx="2655093" cy="674687"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285976</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>81110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>442813</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>68016</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Pravá složená závorka 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CC6F7B3-CCE4-487B-99E4-B5262871C079}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="4531867">
+          <a:off x="799566" y="3401333"/>
+          <a:ext cx="352031" cy="1379212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 44795"/>
+            <a:gd name="adj2" fmla="val 50118"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="cs-CZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>115094</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>51593</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>132522</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextovéPole 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8061476A-0B96-D136-AE36-3B00C92A63B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3152051" y="1509332"/>
+          <a:ext cx="1232210" cy="431904"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="2400"/>
+            <a:t>Výška</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>386556</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>100805</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextovéPole 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BE0D43E-1A4B-461A-8211-754CEB0E48FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="997744" y="4049711"/>
+          <a:ext cx="1383506" cy="432594"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="2400"/>
+            <a:t>Hloubka</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>484188</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>261937</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67469</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Přímá spojnice se šipkou 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11FD26D3-2D61-AF83-17DE-192DAF80242C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2928938" y="63500"/>
+          <a:ext cx="388937" cy="369094"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:headEnd w="sm" len="med"/>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219005</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22088</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>96458</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextovéPole 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{935A833E-C055-4EF5-8348-8D8802A7C81A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3255962" y="22638"/>
+          <a:ext cx="1625256" cy="1167124"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="2200" i="1"/>
+            <a:t>Špička hostujícího meče</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>414025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>181355</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="TextovéPole 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F72CD4C-8EB2-4D9B-A794-47F5360F2763}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3450982" y="3163507"/>
+          <a:ext cx="1789147" cy="1573283"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="2200" i="1"/>
+            <a:t>Konec hostujícího</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="cs-CZ" sz="2200" i="1" baseline="0"/>
+            <a:t> meče</a:t>
+          </a:r>
+          <a:endParaRPr lang="cs-CZ" sz="2200" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>511969</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>150813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>468312</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Přímá spojnice se šipkou 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CA1FA8A-86DE-4C10-A66A-8441B787DA47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2956719" y="3436938"/>
+          <a:ext cx="567531" cy="222250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:headEnd w="sm" len="med"/>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2266,7 +3483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5E9BC4-1613-4D8F-908A-F7A6847BDABE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -2275,4 +3492,52 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228D3C76-000D-402D-A825-AE3B3964C432}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B8714D-9C4F-4377-871D-E55B488130BF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1A4440-3C56-4F91-8FF0-D82E73A8AD54}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
5.3 wip - up to 5.3.2
</commit_message>
<xml_diff>
--- a/img/excel/diagrams.xlsx
+++ b/img/excel/diagrams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubahronik\Desktop\Thesis\img\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501B599F-AE9A-4FF8-9870-E5C32FF9BA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B523DBED-3EF7-4C6A-A877-E90CC0814131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{23EAE5E5-F549-4271-837A-78A13B533C97}"/>
   </bookViews>
@@ -3531,7 +3531,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>